<commit_message>
Correct conda activate --no-stack (the 'a' was missing from stack).
</commit_message>
<xml_diff>
--- a/SyntaxTreeTools/CondaCompletionsSpec 2022-08-13.xlsx
+++ b/SyntaxTreeTools/CondaCompletionsSpec 2022-08-13.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\csharp\POSH-Resolve-Argument\Conda-help-files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\csharp\POSH-Resolve-Argument\SyntaxTreeTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB74779-15B0-49DE-9F0F-F67E0B81E7FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E656F081-429F-40C0-BA36-DAB906E63D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CondaCommands" sheetId="3" r:id="rId1"/>
@@ -1081,9 +1081,6 @@
     <t>Do not stack the environment.</t>
   </si>
   <si>
-    <t>--no-stck</t>
-  </si>
-  <si>
     <t>Deactivate a conda environment.</t>
   </si>
   <si>
@@ -1091,13 +1088,16 @@
   </si>
   <si>
     <t>conda.deactivate</t>
+  </si>
+  <si>
+    <t>--no-stack</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1231,12 +1231,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1580,11 +1574,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1960,24 +1952,24 @@
   <dimension ref="A1:I335"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="20.73046875" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.59765625" customWidth="1"/>
-    <col min="7" max="7" width="14.86328125" customWidth="1"/>
-    <col min="8" max="8" width="15.73046875" customWidth="1"/>
-    <col min="9" max="9" width="71.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="71.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>221</v>
       </c>
@@ -1993,7 +1985,7 @@
       <c r="E1" t="s">
         <v>283</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" t="s">
         <v>309</v>
       </c>
       <c r="G1" t="s">
@@ -2006,7 +1998,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -2019,14 +2011,14 @@
       <c r="D2" t="s">
         <v>334</v>
       </c>
-      <c r="F2" s="3" t="b">
+      <c r="F2" t="b">
         <v>0</v>
       </c>
       <c r="I2" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>134</v>
       </c>
@@ -2046,7 +2038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>134</v>
       </c>
@@ -2066,7 +2058,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>134</v>
       </c>
@@ -2086,7 +2078,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>134</v>
       </c>
@@ -2106,7 +2098,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>134</v>
       </c>
@@ -2117,16 +2109,16 @@
         <v>221</v>
       </c>
       <c r="D7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>134</v>
       </c>
@@ -2146,7 +2138,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>134</v>
       </c>
@@ -2166,7 +2158,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>134</v>
       </c>
@@ -2186,7 +2178,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>134</v>
       </c>
@@ -2206,7 +2198,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>134</v>
       </c>
@@ -2226,7 +2218,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>134</v>
       </c>
@@ -2246,7 +2238,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>134</v>
       </c>
@@ -2266,7 +2258,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>134</v>
       </c>
@@ -2289,7 +2281,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>134</v>
       </c>
@@ -2309,7 +2301,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>134</v>
       </c>
@@ -2329,7 +2321,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>134</v>
       </c>
@@ -2352,7 +2344,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>134</v>
       </c>
@@ -2377,7 +2369,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>134</v>
       </c>
@@ -2402,7 +2394,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>334</v>
       </c>
@@ -2427,7 +2419,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>334</v>
       </c>
@@ -2450,7 +2442,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>334</v>
       </c>
@@ -2461,7 +2453,7 @@
         <v>281</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" t="b">
@@ -2473,7 +2465,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>334</v>
       </c>
@@ -2498,7 +2490,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -2523,7 +2515,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -2548,7 +2540,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -2573,7 +2565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -2598,7 +2590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -2623,7 +2615,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -2648,7 +2640,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -2677,7 +2669,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -2704,7 +2696,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -2727,7 +2719,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -2754,7 +2746,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>48</v>
       </c>
@@ -2781,7 +2773,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>48</v>
       </c>
@@ -2808,7 +2800,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -2831,7 +2823,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>49</v>
       </c>
@@ -2858,7 +2850,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>49</v>
       </c>
@@ -2881,7 +2873,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>49</v>
       </c>
@@ -2908,7 +2900,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -2937,7 +2929,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>49</v>
       </c>
@@ -2966,7 +2958,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>50</v>
       </c>
@@ -2993,7 +2985,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>50</v>
       </c>
@@ -3016,7 +3008,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -3043,7 +3035,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -3070,7 +3062,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -3093,7 +3085,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>50</v>
       </c>
@@ -3116,7 +3108,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -3142,7 +3134,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -3168,7 +3160,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -3191,7 +3183,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -3214,7 +3206,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -3240,7 +3232,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>50</v>
       </c>
@@ -3263,7 +3255,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>50</v>
       </c>
@@ -3289,7 +3281,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>50</v>
       </c>
@@ -3315,7 +3307,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>50</v>
       </c>
@@ -3341,7 +3333,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>50</v>
       </c>
@@ -3368,7 +3360,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>50</v>
       </c>
@@ -3394,7 +3386,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>50</v>
       </c>
@@ -3420,7 +3412,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>50</v>
       </c>
@@ -3446,7 +3438,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>50</v>
       </c>
@@ -3469,7 +3461,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>51</v>
       </c>
@@ -3492,7 +3484,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>51</v>
       </c>
@@ -3519,7 +3511,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>51</v>
       </c>
@@ -3545,7 +3537,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>51</v>
       </c>
@@ -3571,7 +3563,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>51</v>
       </c>
@@ -3594,7 +3586,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>51</v>
       </c>
@@ -3623,7 +3615,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>51</v>
       </c>
@@ -3652,7 +3644,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>51</v>
       </c>
@@ -3681,7 +3673,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>51</v>
       </c>
@@ -3704,7 +3696,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>51</v>
       </c>
@@ -3727,7 +3719,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>51</v>
       </c>
@@ -3753,7 +3745,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>51</v>
       </c>
@@ -3776,7 +3768,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>51</v>
       </c>
@@ -3799,7 +3791,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>51</v>
       </c>
@@ -3822,7 +3814,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>51</v>
       </c>
@@ -3845,7 +3837,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>51</v>
       </c>
@@ -3868,7 +3860,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>51</v>
       </c>
@@ -3891,7 +3883,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>51</v>
       </c>
@@ -3917,7 +3909,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>51</v>
       </c>
@@ -3940,7 +3932,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>51</v>
       </c>
@@ -3963,7 +3955,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>51</v>
       </c>
@@ -3990,7 +3982,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>51</v>
       </c>
@@ -4017,7 +4009,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>51</v>
       </c>
@@ -4040,7 +4032,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>51</v>
       </c>
@@ -4067,7 +4059,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>51</v>
       </c>
@@ -4090,7 +4082,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>51</v>
       </c>
@@ -4117,7 +4109,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>51</v>
       </c>
@@ -4144,7 +4136,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>51</v>
       </c>
@@ -4171,7 +4163,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>51</v>
       </c>
@@ -4194,7 +4186,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>51</v>
       </c>
@@ -4217,12 +4209,12 @@
         <v>119</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>341</v>
+      </c>
+      <c r="B93" t="s">
         <v>342</v>
-      </c>
-      <c r="B93" t="s">
-        <v>343</v>
       </c>
       <c r="C93" t="s">
         <v>280</v>
@@ -4241,7 +4233,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>53</v>
       </c>
@@ -4268,7 +4260,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>53</v>
       </c>
@@ -4295,7 +4287,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>53</v>
       </c>
@@ -4318,7 +4310,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>53</v>
       </c>
@@ -4345,7 +4337,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>53</v>
       </c>
@@ -4368,11 +4360,11 @@
       <c r="H98" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="I98" s="4" t="s">
+      <c r="I98" s="2" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>53</v>
       </c>
@@ -4395,7 +4387,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>53</v>
       </c>
@@ -4418,7 +4410,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>53</v>
       </c>
@@ -4444,7 +4436,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>53</v>
       </c>
@@ -4471,7 +4463,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>54</v>
       </c>
@@ -4494,7 +4486,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>54</v>
       </c>
@@ -4521,7 +4513,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>54</v>
       </c>
@@ -4544,7 +4536,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>54</v>
       </c>
@@ -4567,7 +4559,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>54</v>
       </c>
@@ -4594,7 +4586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>54</v>
       </c>
@@ -4617,7 +4609,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>54</v>
       </c>
@@ -4640,7 +4632,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>54</v>
       </c>
@@ -4666,7 +4658,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>54</v>
       </c>
@@ -4693,7 +4685,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>55</v>
       </c>
@@ -4716,7 +4708,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>55</v>
       </c>
@@ -4743,7 +4735,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>55</v>
       </c>
@@ -4769,7 +4761,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>55</v>
       </c>
@@ -4795,7 +4787,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>55</v>
       </c>
@@ -4818,7 +4810,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>55</v>
       </c>
@@ -4847,7 +4839,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>55</v>
       </c>
@@ -4876,7 +4868,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>55</v>
       </c>
@@ -4905,7 +4897,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>55</v>
       </c>
@@ -4928,7 +4920,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>55</v>
       </c>
@@ -4951,7 +4943,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>55</v>
       </c>
@@ -4977,7 +4969,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>55</v>
       </c>
@@ -5000,7 +4992,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>55</v>
       </c>
@@ -5023,7 +5015,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>55</v>
       </c>
@@ -5046,7 +5038,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>55</v>
       </c>
@@ -5069,7 +5061,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>55</v>
       </c>
@@ -5092,7 +5084,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>55</v>
       </c>
@@ -5118,7 +5110,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>55</v>
       </c>
@@ -5141,7 +5133,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>55</v>
       </c>
@@ -5165,7 +5157,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>55</v>
       </c>
@@ -5175,7 +5167,7 @@
       <c r="C131" t="s">
         <v>281</v>
       </c>
-      <c r="D131" s="2" t="s">
+      <c r="D131" s="1" t="s">
         <v>162</v>
       </c>
       <c r="E131" s="1"/>
@@ -5190,7 +5182,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>55</v>
       </c>
@@ -5213,7 +5205,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>55</v>
       </c>
@@ -5240,7 +5232,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>55</v>
       </c>
@@ -5264,7 +5256,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>55</v>
       </c>
@@ -5289,7 +5281,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>55</v>
       </c>
@@ -5312,7 +5304,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>55</v>
       </c>
@@ -5335,7 +5327,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>55</v>
       </c>
@@ -5358,7 +5350,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>55</v>
       </c>
@@ -5385,7 +5377,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>55</v>
       </c>
@@ -5408,7 +5400,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>55</v>
       </c>
@@ -5435,7 +5427,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>55</v>
       </c>
@@ -5462,7 +5454,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>55</v>
       </c>
@@ -5485,7 +5477,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>55</v>
       </c>
@@ -5512,7 +5504,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>55</v>
       </c>
@@ -5535,7 +5527,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>55</v>
       </c>
@@ -5562,7 +5554,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>55</v>
       </c>
@@ -5589,7 +5581,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>55</v>
       </c>
@@ -5616,7 +5608,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>55</v>
       </c>
@@ -5639,7 +5631,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>55</v>
       </c>
@@ -5662,7 +5654,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>56</v>
       </c>
@@ -5685,7 +5677,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>56</v>
       </c>
@@ -5712,7 +5704,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>56</v>
       </c>
@@ -5735,7 +5727,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>56</v>
       </c>
@@ -5762,7 +5754,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>56</v>
       </c>
@@ -5789,7 +5781,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>56</v>
       </c>
@@ -5812,7 +5804,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>56</v>
       </c>
@@ -5835,7 +5827,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>56</v>
       </c>
@@ -5862,7 +5854,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>56</v>
       </c>
@@ -5889,7 +5881,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>56</v>
       </c>
@@ -5912,7 +5904,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>56</v>
       </c>
@@ -5941,7 +5933,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>56</v>
       </c>
@@ -5970,7 +5962,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>56</v>
       </c>
@@ -5993,7 +5985,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>56</v>
       </c>
@@ -6019,7 +6011,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>56</v>
       </c>
@@ -6046,7 +6038,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>57</v>
       </c>
@@ -6073,7 +6065,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>57</v>
       </c>
@@ -6102,7 +6094,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>57</v>
       </c>
@@ -6129,7 +6121,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>57</v>
       </c>
@@ -6156,7 +6148,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>57</v>
       </c>
@@ -6182,7 +6174,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>57</v>
       </c>
@@ -6208,7 +6200,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>57</v>
       </c>
@@ -6234,7 +6226,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>57</v>
       </c>
@@ -6263,7 +6255,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>57</v>
       </c>
@@ -6292,7 +6284,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>58</v>
       </c>
@@ -6315,7 +6307,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>58</v>
       </c>
@@ -6342,7 +6334,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>58</v>
       </c>
@@ -6365,7 +6357,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>58</v>
       </c>
@@ -6394,7 +6386,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>58</v>
       </c>
@@ -6423,7 +6415,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>58</v>
       </c>
@@ -6452,7 +6444,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>58</v>
       </c>
@@ -6475,7 +6467,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>58</v>
       </c>
@@ -6498,7 +6490,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>58</v>
       </c>
@@ -6524,7 +6516,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>58</v>
       </c>
@@ -6547,7 +6539,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>58</v>
       </c>
@@ -6570,7 +6562,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>58</v>
       </c>
@@ -6594,7 +6586,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>58</v>
       </c>
@@ -6619,7 +6611,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>58</v>
       </c>
@@ -6642,7 +6634,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>58</v>
       </c>
@@ -6668,7 +6660,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>58</v>
       </c>
@@ -6694,7 +6686,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>58</v>
       </c>
@@ -6720,7 +6712,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>58</v>
       </c>
@@ -6743,7 +6735,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>58</v>
       </c>
@@ -6769,7 +6761,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>58</v>
       </c>
@@ -6792,7 +6784,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>58</v>
       </c>
@@ -6818,7 +6810,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>58</v>
       </c>
@@ -6844,7 +6836,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>58</v>
       </c>
@@ -6871,7 +6863,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>60</v>
       </c>
@@ -6894,7 +6886,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>60</v>
       </c>
@@ -6921,7 +6913,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>60</v>
       </c>
@@ -6947,7 +6939,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>60</v>
       </c>
@@ -6970,7 +6962,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>60</v>
       </c>
@@ -6993,7 +6985,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>60</v>
       </c>
@@ -7019,7 +7011,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>60</v>
       </c>
@@ -7042,7 +7034,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>60</v>
       </c>
@@ -7065,7 +7057,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>60</v>
       </c>
@@ -7094,7 +7086,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>60</v>
       </c>
@@ -7123,7 +7115,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>61</v>
       </c>
@@ -7150,7 +7142,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>61</v>
       </c>
@@ -7173,7 +7165,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>61</v>
       </c>
@@ -7200,7 +7192,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>61</v>
       </c>
@@ -7226,7 +7218,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>61</v>
       </c>
@@ -7252,7 +7244,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>61</v>
       </c>
@@ -7281,7 +7273,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>61</v>
       </c>
@@ -7304,7 +7296,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>61</v>
       </c>
@@ -7327,7 +7319,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>61</v>
       </c>
@@ -7353,7 +7345,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>61</v>
       </c>
@@ -7379,7 +7371,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>61</v>
       </c>
@@ -7405,7 +7397,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>61</v>
       </c>
@@ -7428,7 +7420,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>61</v>
       </c>
@@ -7451,7 +7443,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>61</v>
       </c>
@@ -7477,7 +7469,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>61</v>
       </c>
@@ -7503,7 +7495,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>62</v>
       </c>
@@ -7526,7 +7518,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>62</v>
       </c>
@@ -7553,7 +7545,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>62</v>
       </c>
@@ -7579,7 +7571,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>62</v>
       </c>
@@ -7608,7 +7600,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>62</v>
       </c>
@@ -7637,7 +7629,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>62</v>
       </c>
@@ -7666,7 +7658,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>62</v>
       </c>
@@ -7689,7 +7681,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>62</v>
       </c>
@@ -7712,7 +7704,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>62</v>
       </c>
@@ -7738,7 +7730,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>62</v>
       </c>
@@ -7761,7 +7753,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>62</v>
       </c>
@@ -7784,7 +7776,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>62</v>
       </c>
@@ -7807,7 +7799,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>62</v>
       </c>
@@ -7830,7 +7822,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>62</v>
       </c>
@@ -7853,7 +7845,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>62</v>
       </c>
@@ -7879,7 +7871,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>62</v>
       </c>
@@ -7902,7 +7894,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>62</v>
       </c>
@@ -7925,7 +7917,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>62</v>
       </c>
@@ -7948,7 +7940,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>62</v>
       </c>
@@ -7971,7 +7963,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>62</v>
       </c>
@@ -7997,7 +7989,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>62</v>
       </c>
@@ -8020,7 +8012,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>62</v>
       </c>
@@ -8043,7 +8035,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>62</v>
       </c>
@@ -8066,7 +8058,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>62</v>
       </c>
@@ -8089,7 +8081,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>62</v>
       </c>
@@ -8112,7 +8104,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>62</v>
       </c>
@@ -8135,7 +8127,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>62</v>
       </c>
@@ -8161,7 +8153,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>62</v>
       </c>
@@ -8187,7 +8179,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>62</v>
       </c>
@@ -8210,7 +8202,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>62</v>
       </c>
@@ -8236,7 +8228,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>62</v>
       </c>
@@ -8259,7 +8251,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>62</v>
       </c>
@@ -8286,7 +8278,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>62</v>
       </c>
@@ -8312,7 +8304,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>62</v>
       </c>
@@ -8338,7 +8330,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>62</v>
       </c>
@@ -8361,7 +8353,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>62</v>
       </c>
@@ -8384,7 +8376,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>99</v>
       </c>
@@ -8407,7 +8399,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>99</v>
       </c>
@@ -8430,7 +8422,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>99</v>
       </c>
@@ -8453,7 +8445,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>99</v>
       </c>
@@ -8476,7 +8468,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>99</v>
       </c>
@@ -8499,7 +8491,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>99</v>
       </c>
@@ -8522,7 +8514,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>51</v>
       </c>
@@ -8548,7 +8540,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>51</v>
       </c>
@@ -8571,7 +8563,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>51</v>
       </c>
@@ -8597,7 +8589,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>51</v>
       </c>
@@ -8626,7 +8618,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>51</v>
       </c>
@@ -8649,7 +8641,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>51</v>
       </c>
@@ -8675,7 +8667,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>51</v>
       </c>
@@ -8698,7 +8690,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>51</v>
       </c>
@@ -8724,7 +8716,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>51</v>
       </c>
@@ -8753,7 +8745,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>51</v>
       </c>
@@ -8782,7 +8774,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>51</v>
       </c>
@@ -8808,7 +8800,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>51</v>
       </c>
@@ -8834,7 +8826,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>51</v>
       </c>
@@ -8857,7 +8849,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>51</v>
       </c>
@@ -8880,7 +8872,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>51</v>
       </c>
@@ -8906,7 +8898,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>51</v>
       </c>
@@ -8932,7 +8924,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>251</v>
       </c>
@@ -8958,7 +8950,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>251</v>
       </c>
@@ -8987,7 +8979,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>251</v>
       </c>
@@ -9010,7 +9002,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>251</v>
       </c>
@@ -9039,7 +9031,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>251</v>
       </c>
@@ -9062,7 +9054,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>251</v>
       </c>
@@ -9085,7 +9077,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>251</v>
       </c>
@@ -9108,7 +9100,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>251</v>
       </c>
@@ -9137,7 +9129,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="289" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="289" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>251</v>
       </c>
@@ -9166,7 +9158,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="290" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="290" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>251</v>
       </c>
@@ -9189,7 +9181,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="291" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="291" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>251</v>
       </c>
@@ -9215,7 +9207,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="292" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="292" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>251</v>
       </c>
@@ -9241,7 +9233,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="293" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="293" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>56</v>
       </c>
@@ -9267,7 +9259,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="294" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="294" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>56</v>
       </c>
@@ -9290,7 +9282,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="295" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="295" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>56</v>
       </c>
@@ -9316,7 +9308,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="296" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>56</v>
       </c>
@@ -9342,7 +9334,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="297" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="297" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>58</v>
       </c>
@@ -9368,7 +9360,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="298" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="298" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>58</v>
       </c>
@@ -9394,7 +9386,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="299" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="299" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>58</v>
       </c>
@@ -9423,7 +9415,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="300" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="300" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>58</v>
       </c>
@@ -9452,7 +9444,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="301" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="301" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>58</v>
       </c>
@@ -9478,7 +9470,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="302" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="302" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>58</v>
       </c>
@@ -9501,7 +9493,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="303" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="303" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>58</v>
       </c>
@@ -9527,7 +9519,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="304" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="304" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>58</v>
       </c>
@@ -9553,7 +9545,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="305" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="305" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>58</v>
       </c>
@@ -9579,7 +9571,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="306" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="306" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>62</v>
       </c>
@@ -9602,7 +9594,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="307" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="307" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>62</v>
       </c>
@@ -9628,7 +9620,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="308" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="308" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>62</v>
       </c>
@@ -9657,7 +9649,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="309" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="309" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>62</v>
       </c>
@@ -9680,7 +9672,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="310" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="310" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>62</v>
       </c>
@@ -9706,7 +9698,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="311" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="311" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>62</v>
       </c>
@@ -9735,7 +9727,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="312" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="312" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>62</v>
       </c>
@@ -9764,7 +9756,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="313" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="313" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>62</v>
       </c>
@@ -9787,7 +9779,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="314" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="314" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>62</v>
       </c>
@@ -9813,7 +9805,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="315" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="315" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>62</v>
       </c>
@@ -9839,7 +9831,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="316" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="316" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>50</v>
       </c>
@@ -9862,7 +9854,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="317" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="317" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>50</v>
       </c>
@@ -9888,7 +9880,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="318" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="318" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>270</v>
       </c>
@@ -9911,7 +9903,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="319" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="319" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>270</v>
       </c>
@@ -9934,7 +9926,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="320" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="320" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>270</v>
       </c>
@@ -9957,7 +9949,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="321" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="321" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>270</v>
       </c>
@@ -9983,7 +9975,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="322" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="322" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>56</v>
       </c>
@@ -10009,7 +10001,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="323" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="323" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>56</v>
       </c>
@@ -10038,7 +10030,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="324" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="324" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>56</v>
       </c>
@@ -10067,7 +10059,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="325" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="325" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>56</v>
       </c>
@@ -10090,7 +10082,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="326" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="326" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>56</v>
       </c>
@@ -10116,7 +10108,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="327" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="327" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>56</v>
       </c>
@@ -10142,7 +10134,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="328" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="328" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>261</v>
       </c>
@@ -10165,7 +10157,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="329" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="329" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>261</v>
       </c>
@@ -10191,7 +10183,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="330" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="330" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>261</v>
       </c>
@@ -10220,7 +10212,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="331" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="331" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>261</v>
       </c>
@@ -10249,7 +10241,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="332" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="332" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>262</v>
       </c>
@@ -10272,7 +10264,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="333" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="333" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>262</v>
       </c>
@@ -10298,7 +10290,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="334" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="334" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>262</v>
       </c>
@@ -10327,7 +10319,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="335" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="335" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>262</v>
       </c>

</xml_diff>